<commit_message>
Revert "log4j2 logger commit"
This reverts commit 996d8294f1f8e75b2304342023194626e400fd5c.
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/SaucedemoTestExecution.xlsx
+++ b/src/test/resources/testdata/SaucedemoTestExecution.xlsx
@@ -8,23 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Library\I - Jan - March Automation\LoginModulesAutomation\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49662DC3-C7D7-41DF-A24F-675C4259B76C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44B9C941-274F-4635-9638-30EC672B6780}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15990" firstSheet="6" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="VersionHistory" sheetId="4" r:id="rId1"/>
     <sheet name="Testscenarios" sheetId="5" r:id="rId2"/>
-    <sheet name="setUp" sheetId="13" r:id="rId3"/>
-    <sheet name="LoginTestcase" sheetId="6" r:id="rId4"/>
-    <sheet name="SortingTestcases" sheetId="7" r:id="rId5"/>
-    <sheet name="AddToCartTestCases" sheetId="10" r:id="rId6"/>
-    <sheet name="CheckoutTestcases" sheetId="12" r:id="rId7"/>
-    <sheet name="LoginStandard_user" sheetId="11" r:id="rId8"/>
-    <sheet name="verifyLoginInvalidCredentials" sheetId="1" r:id="rId9"/>
-    <sheet name="verifyLandingPagesValidUsers" sheetId="2" r:id="rId10"/>
-    <sheet name="verifyLandingPagesInvalidUser" sheetId="3" r:id="rId11"/>
-    <sheet name="verifySorting" sheetId="9" r:id="rId12"/>
+    <sheet name="LoginTestcase" sheetId="6" r:id="rId3"/>
+    <sheet name="Sorting" sheetId="7" r:id="rId4"/>
+    <sheet name="AddToCart" sheetId="10" r:id="rId5"/>
+    <sheet name="LoginStandard_user" sheetId="11" r:id="rId6"/>
+    <sheet name="verifyEmailFieldFormat" sheetId="1" r:id="rId7"/>
+    <sheet name="verifyLandingPages" sheetId="2" r:id="rId8"/>
+    <sheet name="verifyLandingPagesInvalidUser" sheetId="3" r:id="rId9"/>
+    <sheet name="verifySorting" sheetId="9" r:id="rId10"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -36,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="96">
   <si>
     <t>username</t>
   </si>
@@ -62,6 +60,15 @@
     <t>problem_user</t>
   </si>
   <si>
+    <t>performance_glitch_user</t>
+  </si>
+  <si>
+    <t>error_user</t>
+  </si>
+  <si>
+    <t>visual_user</t>
+  </si>
+  <si>
     <t>locked_out_user</t>
   </si>
   <si>
@@ -123,6 +130,12 @@
   </si>
   <si>
     <t>Verfity the login functionlaity.</t>
+  </si>
+  <si>
+    <t>Verify deleting items from shopping cart via Product page.</t>
+  </si>
+  <si>
+    <t>Verify the logout functionality.</t>
   </si>
   <si>
     <t>Verify the checkout functionality.</t>
@@ -283,7 +296,13 @@
     <t>TS-002 : Sort functionlaity</t>
   </si>
   <si>
+    <t>TS-007 : Remove item from shoppingcart</t>
+  </si>
+  <si>
     <t>TS-008 : Checkout</t>
+  </si>
+  <si>
+    <t>TS-009 : Logout</t>
   </si>
   <si>
     <t>Sorting Types</t>
@@ -360,37 +379,6 @@
   </si>
   <si>
     <t>Verify that a user can cancel checking out.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. Open the Application URL (https://www.saucedemo.com/) in any supported Browser
-2. Login credentials username/password:standard_user/secret_sauce2. 3.Checkout details FirstName/lastName:checkout_user/testing/Zip:4458
-</t>
-  </si>
-  <si>
-    <t>1. Use credetials in pre-requisite to log into saucedemo.com
-2. On the top right corner click cart icon &amp; remove item in the shopping-cart. credetials in 3. Click shopping cart.
-4. In the shopping cart, click finish button.                    5.  Enter checkout details provided in pre-requisite.                                                                                 6.  Click continue.                                                                     7. Click finish.</t>
-  </si>
-  <si>
-    <t>1. Thank you message.</t>
-  </si>
-  <si>
-    <t>Browser Name</t>
-  </si>
-  <si>
-    <t>firefox</t>
-  </si>
-  <si>
-    <t>chrome</t>
-  </si>
-  <si>
-    <t>edge</t>
-  </si>
-  <si>
-    <t>error_user</t>
-  </si>
-  <si>
-    <t>visual_user</t>
   </si>
 </sst>
 </file>
@@ -491,7 +479,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -502,6 +490,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -824,37 +815,37 @@
   <sheetData>
     <row r="15" spans="12:13" x14ac:dyDescent="0.25">
       <c r="L15" s="3" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="M15" s="4" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
     </row>
     <row r="16" spans="12:13" x14ac:dyDescent="0.25">
       <c r="L16" s="3" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="M16" s="4" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
     </row>
     <row r="17" spans="12:13" x14ac:dyDescent="0.25">
       <c r="L17" s="3" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="M17" s="5" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
     </row>
     <row r="18" spans="12:13" x14ac:dyDescent="0.25">
       <c r="L18" s="3" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="M18" s="5"/>
     </row>
     <row r="19" spans="12:13" x14ac:dyDescent="0.25">
       <c r="L19" s="2" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="M19" s="5"/>
     </row>
@@ -868,100 +859,6 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{082BDED4-2B82-4B47-8A0B-A02EDF57EF93}">
-  <dimension ref="A1:B5"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="10.140625" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>96</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>97</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D97DC781-F51F-4DE5-AD85-BEA3F457E766}">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{288F3A01-2240-4D2E-B39D-8733F2D0C5B4}">
   <dimension ref="A1:A5"/>
   <sheetViews>
@@ -973,28 +870,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
-        <v>67</v>
+      <c r="A1" s="17" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>68</v>
+        <v>75</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>71</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -1004,10 +901,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BEBE3EBE-E3E9-491E-A9DA-AFA7C7AC27FA}">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1021,39 +918,39 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B5" s="6">
         <v>45306</v>
@@ -1061,7 +958,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B6" s="6">
         <v>45322</v>
@@ -1069,83 +966,103 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>85</v>
+        <v>92</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="D10" s="5"/>
       <c r="E10" s="7"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>85</v>
+        <v>92</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="D11" s="5"/>
       <c r="E11" s="7"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>86</v>
+        <v>93</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>85</v>
+        <v>92</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="D12" s="5"/>
       <c r="E12" s="7"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>85</v>
-      </c>
+      <c r="A13" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="B13" s="5"/>
       <c r="C13" s="5" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="D13" s="5"/>
       <c r="E13" s="7"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>87</v>
+        <v>72</v>
       </c>
       <c r="B14" s="5"/>
       <c r="C14" s="5" t="s">
-        <v>88</v>
+        <v>34</v>
       </c>
       <c r="D14" s="5"/>
       <c r="E14" s="7"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="D15" s="5"/>
+      <c r="E15" s="7"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="B16" s="5"/>
+      <c r="C16" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D16" s="5"/>
+      <c r="E16" s="7"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1154,208 +1071,169 @@
     <hyperlink ref="B10" location="LoginTestcase!A1" display="Testcases" xr:uid="{1BC45C30-FD90-4144-9F62-532808C0E786}"/>
     <hyperlink ref="B11" location="Sorting!A1" display="Testcases" xr:uid="{5E0F9B29-64F5-464F-B133-DA3DEFD4ABF2}"/>
     <hyperlink ref="B12" location="AddToCart!A1" display="Testcases" xr:uid="{519F8A99-A1F7-4042-A16D-501712BF08AC}"/>
-    <hyperlink ref="B13" location="CheckoutTestcases!A1" display="Testcases" xr:uid="{CBEEED7A-E7C4-460E-A4D1-76CDFE8F406C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA46ABFB-CFBF-417B-9845-D033F5CE6B96}">
-  <dimension ref="A1:A4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F0D06BE-88A9-4B3D-A371-621FEC80BC99}">
+  <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>95</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F0D06BE-88A9-4B3D-A371-621FEC80BC99}">
-  <dimension ref="A1:J6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="14.28515625" style="8" customWidth="1"/>
-    <col min="2" max="2" width="24.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="37.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="40.85546875" style="8" customWidth="1"/>
-    <col min="5" max="5" width="46.7109375" style="8" customWidth="1"/>
-    <col min="6" max="6" width="39.140625" style="8" customWidth="1"/>
-    <col min="7" max="7" width="35.140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.28515625" style="9" customWidth="1"/>
+    <col min="2" max="2" width="24.140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="37.140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="40.85546875" style="9" customWidth="1"/>
+    <col min="5" max="5" width="46.7109375" style="9" customWidth="1"/>
+    <col min="6" max="6" width="39.140625" style="9" customWidth="1"/>
+    <col min="7" max="7" width="35.140625" style="9" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="18.140625" customWidth="1"/>
     <col min="9" max="9" width="15" customWidth="1"/>
     <col min="10" max="11" width="13.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="B1" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="C1" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="D1" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="E1" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="F1" s="9" t="s">
+      <c r="A1" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="B2" s="18"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="18"/>
+      <c r="I2" s="18"/>
+      <c r="J2" s="18"/>
+    </row>
+    <row r="3" spans="1:10" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="D3" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="F3" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="G3" s="15" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="D4" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="E4" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="G4" s="13" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="E5" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="F5" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="G5" s="13" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+      <c r="A6" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="C6" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="G1" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="17" t="s">
-        <v>48</v>
-      </c>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17"/>
-      <c r="G2" s="17"/>
-      <c r="H2" s="17"/>
-      <c r="I2" s="17"/>
-      <c r="J2" s="17"/>
-    </row>
-    <row r="3" spans="1:10" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="C3" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="D3" s="12" t="s">
-        <v>81</v>
-      </c>
-      <c r="E3" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="F3" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="G3" s="14" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="B4" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="C4" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="D4" s="14" t="s">
-        <v>82</v>
-      </c>
-      <c r="E4" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="F4" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="G4" s="12" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="75" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="B5" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="C5" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="D5" s="12" t="s">
-        <v>83</v>
-      </c>
-      <c r="E5" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="F5" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="G5" s="12" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="75" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="C6" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="D6" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="E6" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="F6" s="15" t="s">
+      <c r="D6" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="E6" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="G6" s="12" t="s">
-        <v>63</v>
+      <c r="F6" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="G6" s="13" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -1372,7 +1250,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{897176EE-73A7-47AF-B5BE-F9CDBD0A4BDC}">
   <dimension ref="A1:J6"/>
   <sheetViews>
@@ -1392,141 +1270,141 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="B1" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="C1" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="D1" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="E1" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="F1" s="9" t="s">
+      <c r="A1" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="B2" s="18"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="18"/>
+      <c r="I2" s="18"/>
+      <c r="J2" s="18"/>
+    </row>
+    <row r="3" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="D3" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="F3" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="G3" s="15" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="D4" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="E4" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="G4" s="13" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="E5" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="F5" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="G5" s="13" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="68.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="C6" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="G1" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="17" t="s">
-        <v>48</v>
-      </c>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17"/>
-      <c r="G2" s="17"/>
-      <c r="H2" s="17"/>
-      <c r="I2" s="17"/>
-      <c r="J2" s="17"/>
-    </row>
-    <row r="3" spans="1:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="C3" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="D3" s="12" t="s">
-        <v>81</v>
-      </c>
-      <c r="E3" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="F3" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="G3" s="14" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="B4" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="C4" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="D4" s="14" t="s">
-        <v>82</v>
-      </c>
-      <c r="E4" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="F4" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="G4" s="12" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="B5" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="C5" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="D5" s="12" t="s">
-        <v>83</v>
-      </c>
-      <c r="E5" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="F5" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="G5" s="12" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="68.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="C6" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="D6" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="E6" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="F6" s="15" t="s">
+      <c r="D6" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="E6" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="G6" s="12" t="s">
-        <v>63</v>
+      <c r="F6" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="G6" s="13" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -1543,12 +1421,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89958BCA-3295-4FF0-8FB9-B3948AEE8CA7}">
   <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:J6"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1566,141 +1444,141 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="B1" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="C1" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="D1" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="E1" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="F1" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="G1" s="9" t="s">
+      <c r="A1" s="10" t="s">
         <v>35</v>
       </c>
+      <c r="B1" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>40</v>
+      </c>
       <c r="H1" s="2" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="B2" s="18"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="18"/>
+      <c r="I2" s="18"/>
+      <c r="J2" s="18"/>
+    </row>
+    <row r="3" spans="1:10" ht="105" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="D3" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="F3" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="G3" s="15" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="105" x14ac:dyDescent="0.25">
+      <c r="A4" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17"/>
-      <c r="G2" s="17"/>
-      <c r="H2" s="17"/>
-      <c r="I2" s="17"/>
-      <c r="J2" s="17"/>
-    </row>
-    <row r="3" spans="1:10" ht="105" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="C3" s="10" t="s">
-        <v>72</v>
-      </c>
-      <c r="D3" s="12" t="s">
+      <c r="B4" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="E3" s="12" t="s">
-        <v>76</v>
-      </c>
-      <c r="F3" s="13" t="s">
+      <c r="D4" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="E4" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="G4" s="13" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="105" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="G3" s="14" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="105" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="B4" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="C4" s="11" t="s">
-        <v>73</v>
-      </c>
-      <c r="D4" s="12" t="s">
-        <v>80</v>
-      </c>
-      <c r="E4" s="12" t="s">
-        <v>77</v>
-      </c>
-      <c r="F4" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="G4" s="12" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="105" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="B5" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="C5" s="11" t="s">
-        <v>74</v>
-      </c>
-      <c r="D5" s="12" t="s">
-        <v>80</v>
-      </c>
-      <c r="E5" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="F5" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="G5" s="12" t="s">
-        <v>61</v>
+      <c r="B5" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="E5" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="F5" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="G5" s="13" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="105" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="C6" s="11" t="s">
-        <v>75</v>
-      </c>
-      <c r="D6" s="12" t="s">
-        <v>80</v>
-      </c>
-      <c r="E6" s="12" t="s">
-        <v>79</v>
-      </c>
-      <c r="F6" s="15" t="s">
-        <v>62</v>
-      </c>
-      <c r="G6" s="12" t="s">
-        <v>63</v>
+      <c r="A6" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="E6" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="F6" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="G6" s="13" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -1717,181 +1595,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05E5F820-B263-45A1-9392-DAF04714928E}">
-  <dimension ref="A1:J6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:J2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="49.140625" customWidth="1"/>
-    <col min="5" max="5" width="46.85546875" customWidth="1"/>
-    <col min="6" max="6" width="28.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="32.140625" customWidth="1"/>
-    <col min="8" max="8" width="15.85546875" customWidth="1"/>
-    <col min="9" max="9" width="15.7109375" customWidth="1"/>
-    <col min="10" max="10" width="13.140625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="B1" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="C1" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="D1" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="E1" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="F1" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="G1" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="17" t="s">
-        <v>48</v>
-      </c>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17"/>
-      <c r="G2" s="17"/>
-      <c r="H2" s="17"/>
-      <c r="I2" s="17"/>
-      <c r="J2" s="17"/>
-    </row>
-    <row r="3" spans="1:10" ht="90" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="C3" s="10" t="s">
-        <v>72</v>
-      </c>
-      <c r="D3" s="12" t="s">
-        <v>80</v>
-      </c>
-      <c r="E3" s="12" t="s">
-        <v>76</v>
-      </c>
-      <c r="F3" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="G3" s="14" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="150" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="B4" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="C4" s="11" t="s">
-        <v>73</v>
-      </c>
-      <c r="D4" s="12" t="s">
-        <v>89</v>
-      </c>
-      <c r="E4" s="12" t="s">
-        <v>90</v>
-      </c>
-      <c r="F4" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="G4" s="12" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="90" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="B5" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="C5" s="11" t="s">
-        <v>74</v>
-      </c>
-      <c r="D5" s="12" t="s">
-        <v>80</v>
-      </c>
-      <c r="E5" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="F5" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="G5" s="12" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="90" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="C6" s="11" t="s">
-        <v>75</v>
-      </c>
-      <c r="D6" s="12" t="s">
-        <v>80</v>
-      </c>
-      <c r="E6" s="12" t="s">
-        <v>79</v>
-      </c>
-      <c r="F6" s="15" t="s">
-        <v>62</v>
-      </c>
-      <c r="G6" s="12" t="s">
-        <v>63</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A2:J2"/>
-  </mergeCells>
-  <hyperlinks>
-    <hyperlink ref="A2:J2" location="Testscenarios!A1" display="Test scenarios" xr:uid="{23865F35-1B28-446B-B247-76C7C997A32E}"/>
-    <hyperlink ref="F3" location="verifyEmailFieldFormat!A1" display="verifyEmailFieldFormat" xr:uid="{E2BC5C84-04FB-4666-8488-2BB25A0E5BC2}"/>
-    <hyperlink ref="F5" location="verifyLandingPages!A1" display="verifyLandingPages" xr:uid="{0091D56B-07CF-4101-982A-92A050107634}"/>
-    <hyperlink ref="F6" location="verifyLandingPagesInvalidUser!A1" display="verifyLandingPagesInvalidUser" xr:uid="{0CB41490-D9CE-4AEE-972F-1A6D6A7B3E6A}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39FC7113-2697-4FC2-A4C4-20A7D10D4CC4}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -1926,7 +1630,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
@@ -1973,4 +1677,106 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{082BDED4-2B82-4B47-8A0B-A02EDF57EF93}">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:XFD3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D97DC781-F51F-4DE5-AD85-BEA3F457E766}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>